<commit_message>
Fixed tests for Rows in Reader
</commit_message>
<xml_diff>
--- a/tests/util/excels/1sheet-nheader.xlsx
+++ b/tests/util/excels/1sheet-nheader.xlsx
@@ -47,10 +47,10 @@
     <t>Y Value</t>
   </si>
   <si>
-    <t>First Value</t>
-  </si>
-  <si>
-    <t>Second Value</t>
+    <t>First Entry</t>
+  </si>
+  <si>
+    <t>Second Entry</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A6:D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>